<commit_message>
modifs demandées par JC
</commit_message>
<xml_diff>
--- a/la-cave-de-deuxfoiscinq/carte-des-vins.xlsx
+++ b/la-cave-de-deuxfoiscinq/carte-des-vins.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="27980" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="VIGNERONS" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="123">
   <si>
     <t>rivaz</t>
   </si>
@@ -385,6 +385,18 @@
   </si>
   <si>
     <t>oratorio</t>
+  </si>
+  <si>
+    <t>bofflens</t>
+  </si>
+  <si>
+    <t>christian dugon</t>
+  </si>
+  <si>
+    <t>https://www.dugon.ch</t>
+  </si>
+  <si>
+    <t>symphonie</t>
   </si>
 </sst>
 </file>
@@ -829,8 +841,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau13" displayName="Tableau13" ref="A1:E14" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A1:E14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau13" displayName="Tableau13" ref="A1:E15" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A1:E15"/>
   <tableColumns count="5">
     <tableColumn id="1" name="ID_VIGNERON" dataDxfId="16"/>
     <tableColumn id="4" name="DOMAINE" dataDxfId="15"/>
@@ -843,8 +855,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:J54" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J54"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:J55" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J55"/>
   <tableColumns count="10">
     <tableColumn id="3" name="ID_VIGNERON" dataDxfId="9"/>
     <tableColumn id="1" name="ID_VIN" dataDxfId="8"/>
@@ -1125,10 +1137,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuille1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="169" zoomScaleNormal="169" zoomScalePageLayoutView="169" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="169" zoomScaleNormal="169" zoomScalePageLayoutView="169" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1377,6 +1389,20 @@
       </c>
       <c r="E14" s="6" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
+        <v>-14</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1408,10 +1434,11 @@
   <sheetPr codeName="Feuille2" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="169" zoomScaleNormal="169" zoomScalePageLayoutView="169" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView zoomScale="138" zoomScaleNormal="138" zoomScalePageLayoutView="169" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1422,7 +1449,7 @@
     <col min="4" max="4" width="20.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5" style="2" customWidth="1"/>
     <col min="10" max="10" width="16.1640625" style="6" bestFit="1" customWidth="1"/>
@@ -2829,7 +2856,7 @@
         <v>7.2</v>
       </c>
       <c r="H51" s="4"/>
-      <c r="I51" s="12" t="s">
+      <c r="I51" s="11" t="s">
         <v>115</v>
       </c>
       <c r="J51" s="2"/>
@@ -2857,7 +2884,7 @@
         <v>10</v>
       </c>
       <c r="H52" s="4"/>
-      <c r="I52" s="12" t="s">
+      <c r="I52" s="11" t="s">
         <v>115</v>
       </c>
       <c r="J52" s="2"/>
@@ -2885,7 +2912,7 @@
         <v>20</v>
       </c>
       <c r="H53" s="4"/>
-      <c r="I53" s="12" t="s">
+      <c r="I53" s="11" t="s">
         <v>115</v>
       </c>
       <c r="J53" s="2"/>
@@ -2913,10 +2940,38 @@
         <v>11.25</v>
       </c>
       <c r="H54" s="4"/>
-      <c r="I54" s="12" t="s">
+      <c r="I54" s="11" t="s">
         <v>115</v>
       </c>
       <c r="J54" s="2"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
+        <v>-14</v>
+      </c>
+      <c r="B55" s="2">
+        <v>51</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E55" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G55" s="4">
+        <v>7</v>
+      </c>
+      <c r="H55" s="4"/>
+      <c r="I55" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="J55" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>